<commit_message>
add tented vias to both FMC
</commit_message>
<xml_diff>
--- a/Project Outputs for llrf_fmc_extension/BOM/llrf_fmc_extension.xlsx
+++ b/Project Outputs for llrf_fmc_extension/BOM/llrf_fmc_extension.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YandexDisk\Work\Altium\COSY\llrf_fmc_extention_pcb\Project Outputs for llrf_fmc_extension\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49CBCA2A-355E-48AF-B7E1-95A5D7CFF077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{38AB7D23-8CAA-462F-8EA5-157168D1A2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="5445" windowWidth="28110" windowHeight="15885" xr2:uid="{D1EDD4BB-6F9D-41C2-8832-D8EEE24F20C6}"/>
+    <workbookView xWindow="65145" yWindow="15195" windowWidth="11655" windowHeight="7980" xr2:uid="{E3ED1994-82D1-4D7D-B2B9-B56DEE70BE26}"/>
   </bookViews>
   <sheets>
     <sheet name="llrf_fmc_extension" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -460,22 +462,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB491296-8BAC-4AC0-ABC8-606619C2CC8E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7378A97E-6AF8-4909-8908-AFBF7312737A}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="55.77734375" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="34.21875" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -495,7 +497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -513,7 +515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -531,7 +533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -551,6 +553,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>